<commit_message>
Regretion Run SCD0170, SCD0171, SCD0172, SCD0173, And SCD0176
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0171_Menu BNI Multifinance.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0171_Menu BNI Multifinance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E7DE50-2B8B-4C10-A299-703BC8D16EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DFC94A-B2DE-4EA4-8DDF-B69D7DFDE8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="3615" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0171" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>RUN</t>
   </si>
@@ -133,6 +133,9 @@
  · Car Ownership Program (COP)
  · Motorcycle Ownership Program (MOP)
  · Computer/Laptop Ownership Program (COOP)</t>
+  </si>
+  <si>
+    <t>TEXT3</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,6 +610,9 @@
       </c>
       <c r="M1" t="s">
         <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>